<commit_message>
update field pass energy code
</commit_message>
<xml_diff>
--- a/R/data_refs/refbyhand_fuel.xlsx
+++ b/R/data_refs/refbyhand_fuel.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_refs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EB4BA2-6CDD-4C67-87C8-5A1C2352C13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281EED66-2D36-4498-8F76-5857C6DF126F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31350" yWindow="2220" windowWidth="21600" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="energy" sheetId="1" r:id="rId1"/>
-    <sheet name="combustion-co2" sheetId="2" r:id="rId2"/>
+    <sheet name="conversion-eff" sheetId="3" r:id="rId2"/>
+    <sheet name="combustion-co2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="50">
   <si>
     <t>fuel_type</t>
   </si>
@@ -128,12 +129,6 @@
     <t>Table S3, cites 2006 IPCC report, note they call this embodied energy</t>
   </si>
   <si>
-    <t>Note the btus in one kwh of electricity is a constant</t>
-  </si>
-  <si>
-    <t>google</t>
-  </si>
-  <si>
     <t>IPCC emission factor database</t>
   </si>
   <si>
@@ -159,6 +154,24 @@
   </si>
   <si>
     <t>For stationary combustion</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>MJ/L</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>Hoffman, G.J., T.A. Howell, and K.H. Solomon. 1992.  Management of Farm Irrigation Systems, ASAE Monograph Number 9 .</t>
+  </si>
+  <si>
+    <t>Hoffman et al 1992</t>
+  </si>
+  <si>
+    <t>Table 19.1</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1051,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1094,31 +1107,33 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9">
-        <v>3.6</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>43</v>
+        <v>9.4</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>32</v>
@@ -1126,16 +1141,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11">
-        <v>9.4</v>
+        <v>39.6</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>32</v>
@@ -1143,19 +1158,53 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>39.020000000000003</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12">
-        <v>39.6</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>32</v>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <v>34.56</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>3.6</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1164,6 +1213,88 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC62357-0511-4CA3-B251-33E17DB7C578}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="155" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7">
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9">
+        <v>90.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
@@ -1465,16 +1596,16 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" s="2">
         <v>0.45</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1482,16 +1613,16 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
         <v>37</v>
-      </c>
-      <c r="C24" t="s">
-        <v>39</v>
       </c>
       <c r="D24" s="2">
         <v>0.08</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1499,16 +1630,16 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2">
         <v>3188</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1516,16 +1647,16 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2">
         <v>74100</v>
       </c>
       <c r="E26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1533,16 +1664,16 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="2">
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1550,16 +1681,16 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2">
         <v>0.6</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update fuel manu energy
</commit_message>
<xml_diff>
--- a/R/data_refs/refbyhand_fuel.xlsx
+++ b/R/data_refs/refbyhand_fuel.xlsx
@@ -8,21 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_refs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281EED66-2D36-4498-8F76-5857C6DF126F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A837EE12-CE8B-48D8-82F0-550BB69E667E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31350" yWindow="2220" windowWidth="21600" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4470" yWindow="2355" windowWidth="21600" windowHeight="11325" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="energy" sheetId="1" r:id="rId1"/>
     <sheet name="conversion-eff" sheetId="3" r:id="rId2"/>
-    <sheet name="combustion-co2" sheetId="2" r:id="rId3"/>
+    <sheet name="manufacture" sheetId="4" r:id="rId3"/>
+    <sheet name="electric-by-state" sheetId="5" r:id="rId4"/>
+    <sheet name="combustion-co2" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
   <si>
     <t>fuel_type</t>
   </si>
@@ -172,6 +187,183 @@
   </si>
   <si>
     <t>Table 19.1</t>
+  </si>
+  <si>
+    <t>Comes from GREET database, not sure if it's correct</t>
+  </si>
+  <si>
+    <t>btu/mmbtu</t>
+  </si>
+  <si>
+    <t>greet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line 263 from 'petroleum' tab (feedstock + fuel) </t>
+  </si>
+  <si>
+    <t>line 541 from 'electric' tab, column G (CA specific value)</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>total energy</t>
+  </si>
+  <si>
+    <t>taken from greet1_2022 table, electric tab</t>
   </si>
 </sst>
 </file>
@@ -503,7 +695,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -618,6 +810,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -664,11 +918,24 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1028,7 +1295,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC62357-0511-4CA3-B251-33E17DB7C578}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1295,6 +1562,535 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF36B0A1-B092-49AF-918A-1D20B104DADF}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7">
+        <v>237724</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8">
+        <v>219472</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1751558.4793751165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDE146B-A555-43AD-B911-2FCCB19A3F29}">
+  <dimension ref="A1:B57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2560784.2462715139</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>2042826.4776977412</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>2315928.6631540433</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>2053129.1331972515</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1751558.4793751165</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2498583.5819126591</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1810185.6120852982</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>3480873.5784830092</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2708970.6732206871</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2368074.0208908846</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>2167974.2159522544</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>3421434.3534036186</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>2112887.4540301901</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>1361645.1097872243</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>1920722.3191254092</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>2887203.9595537884</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>1978660.5696144833</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>3009020.9726553056</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>2545956.2017373675</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>2275870.0673133023</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>2077944.8014844544</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2349305.5831553484</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>2313246.6291803513</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>2165363.8588073915</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>2728262.7735934332</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>2319164.5749160685</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>2177451.1085846755</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>2010853.1742216183</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>2591179.0138278934</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>2284335.8700390221</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>1692016.9903794336</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>1799491.3032962172</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>2659886.7605724195</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>2047657.9433959115</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>1814360.7201097221</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>2607767.1673954516</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>2128680.6405651919</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>1429694.3177147498</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>2008779.6560113581</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>2263478.976617225</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>1802663.0673283252</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>1545078.9807206674</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>2001289.2846407986</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>2348803.2827445017</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>2684423.0906548309</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>2050526.5093742481</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>1664321.5142441341</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>1368740.3326246841</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>2618228.5768152177</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>2917258.9577595112</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>2909275.1676287227</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix avoided fert calcs2
</commit_message>
<xml_diff>
--- a/R/data_refs/refbyhand_fuel.xlsx
+++ b/R/data_refs/refbyhand_fuel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_refs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A837EE12-CE8B-48D8-82F0-550BB69E667E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0597EB25-FF27-4B53-BE27-F6BD54F3620E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="2355" windowWidth="21600" windowHeight="11325" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="energy" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
do ghg from energy calcs
</commit_message>
<xml_diff>
--- a/R/data_refs/refbyhand_fuel.xlsx
+++ b/R/data_refs/refbyhand_fuel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_refs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0597EB25-FF27-4B53-BE27-F6BD54F3620E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D01BDDC-281F-4CD0-B0B3-144AC23CB6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="energy" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="107">
   <si>
     <t>fuel_type</t>
   </si>
@@ -60,15 +60,9 @@
     <t>EPA</t>
   </si>
   <si>
-    <t>ca electricity</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>kg co2/gal</t>
-  </si>
-  <si>
     <t>https://www.epa.gov/sites/default/files/2020-12/documents/mobileemissions.pdf; Table A-1</t>
   </si>
   <si>
@@ -90,48 +84,21 @@
     <t>EPA - GHG inventory guidance - direct emissions from mobile combustion souces</t>
   </si>
   <si>
-    <t>lb co2e/MWh</t>
-  </si>
-  <si>
     <t>Grassini and Cassman cite weird things I haven't tracked down yet</t>
   </si>
   <si>
-    <t>kg co2/l</t>
-  </si>
-  <si>
-    <t>kg co2/kwh</t>
-  </si>
-  <si>
     <t>FTM does not include ch4 nor n2o in this, only co2</t>
   </si>
   <si>
-    <t>g ch4/gal</t>
-  </si>
-  <si>
     <t>motor gasoline Table A-1</t>
   </si>
   <si>
     <t>Table B-8</t>
   </si>
   <si>
-    <t>g n2o/gal</t>
-  </si>
-  <si>
     <t xml:space="preserve"> https://www.epa.gov/egrid/summary-data; from 2021 data; not sure if this is only direct emissions or includes indirect emissions</t>
   </si>
   <si>
-    <t>kg n2o/l</t>
-  </si>
-  <si>
-    <t>kg n2o/kwh</t>
-  </si>
-  <si>
-    <t>kg ch4/l</t>
-  </si>
-  <si>
-    <t>kg ch4/kwh</t>
-  </si>
-  <si>
     <t>Grassini and Cassman cite IPCC; https://www.pnas.org/doi/10.1073/pnas.1116364109#supplementary-materials</t>
   </si>
   <si>
@@ -147,27 +114,9 @@
     <t>IPCC emission factor database</t>
   </si>
   <si>
-    <t>g ch4/kg</t>
-  </si>
-  <si>
-    <t>g n2o/kg</t>
-  </si>
-  <si>
-    <t>g co2/kg</t>
-  </si>
-  <si>
     <t>For stationary farm equipment</t>
   </si>
   <si>
-    <t>kg co2/tj</t>
-  </si>
-  <si>
-    <t>kg ch4/tj</t>
-  </si>
-  <si>
-    <t>kg n2o/tj</t>
-  </si>
-  <si>
     <t>For stationary combustion</t>
   </si>
   <si>
@@ -364,6 +313,51 @@
   </si>
   <si>
     <t>taken from greet1_2022 table, electric tab</t>
+  </si>
+  <si>
+    <t>co2</t>
+  </si>
+  <si>
+    <t>ch4</t>
+  </si>
+  <si>
+    <t>n2o</t>
+  </si>
+  <si>
+    <t>co2e</t>
+  </si>
+  <si>
+    <t>kg/gal</t>
+  </si>
+  <si>
+    <t>g/gal</t>
+  </si>
+  <si>
+    <t>lb/MWh</t>
+  </si>
+  <si>
+    <t>kg/l</t>
+  </si>
+  <si>
+    <t>kg/kwh</t>
+  </si>
+  <si>
+    <t>g/kg</t>
+  </si>
+  <si>
+    <t>kg/tj</t>
+  </si>
+  <si>
+    <t>molecule</t>
+  </si>
+  <si>
+    <t>lb/gal</t>
+  </si>
+  <si>
+    <t>FTM</t>
+  </si>
+  <si>
+    <t>lb/kwh</t>
   </si>
 </sst>
 </file>
@@ -1308,17 +1302,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1335,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1346,13 +1340,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>0.13800000000000001</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1363,13 +1357,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>0.125</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1377,33 +1371,33 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
       </c>
       <c r="D9">
         <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>9.4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1411,16 +1405,16 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
       </c>
       <c r="D11">
         <v>39.6</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1428,16 +1422,16 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>39.020000000000003</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1445,33 +1439,33 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>34.56</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14">
         <v>3.6</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1497,7 +1491,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -1519,10 +1513,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>30.3</v>
@@ -1533,10 +1527,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>23.6</v>
@@ -1544,13 +1538,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>90.6</v>
@@ -1576,17 +1570,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1603,7 +1597,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1611,10 +1605,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>237724</v>
@@ -1626,10 +1620,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>219472</v>
@@ -1637,13 +1631,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D9" s="4">
         <v>1751558.4793751165</v>
@@ -1658,7 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDE146B-A555-43AD-B911-2FCCB19A3F29}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1666,15 +1660,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1682,7 +1676,7 @@
         <v>2560784.2462715139</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1690,7 +1684,7 @@
         <v>2042826.4776977412</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1698,7 +1692,7 @@
         <v>2315928.6631540433</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1706,7 +1700,7 @@
         <v>2053129.1331972515</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1714,7 +1708,7 @@
         <v>1751558.4793751165</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1722,7 +1716,7 @@
         <v>2498583.5819126591</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1730,7 +1724,7 @@
         <v>1810185.6120852982</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1738,7 +1732,7 @@
         <v>3480873.5784830092</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1746,7 +1740,7 @@
         <v>2708970.6732206871</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1754,7 +1748,7 @@
         <v>2368074.0208908846</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1762,7 +1756,7 @@
         <v>2167974.2159522544</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1770,7 +1764,7 @@
         <v>3421434.3534036186</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1778,7 +1772,7 @@
         <v>2112887.4540301901</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1786,7 +1780,7 @@
         <v>1361645.1097872243</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1794,7 +1788,7 @@
         <v>1920722.3191254092</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1802,7 +1796,7 @@
         <v>2887203.9595537884</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1810,7 +1804,7 @@
         <v>1978660.5696144833</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1818,7 +1812,7 @@
         <v>3009020.9726553056</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1826,7 +1820,7 @@
         <v>2545956.2017373675</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1834,7 +1828,7 @@
         <v>2275870.0673133023</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1842,7 +1836,7 @@
         <v>2077944.8014844544</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1850,7 +1844,7 @@
         <v>2349305.5831553484</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1858,7 +1852,7 @@
         <v>2313246.6291803513</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1866,7 +1860,7 @@
         <v>2165363.8588073915</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1874,7 +1868,7 @@
         <v>2728262.7735934332</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1882,7 +1876,7 @@
         <v>2319164.5749160685</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1890,7 +1884,7 @@
         <v>2177451.1085846755</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1898,7 +1892,7 @@
         <v>2010853.1742216183</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1906,7 +1900,7 @@
         <v>2591179.0138278934</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1914,7 +1908,7 @@
         <v>2284335.8700390221</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1922,7 +1916,7 @@
         <v>1692016.9903794336</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1930,7 +1924,7 @@
         <v>1799491.3032962172</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1938,7 +1932,7 @@
         <v>2659886.7605724195</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1946,7 +1940,7 @@
         <v>2047657.9433959115</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1954,7 +1948,7 @@
         <v>1814360.7201097221</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1962,7 +1956,7 @@
         <v>2607767.1673954516</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1970,7 +1964,7 @@
         <v>2128680.6405651919</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1978,7 +1972,7 @@
         <v>1429694.3177147498</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1986,7 +1980,7 @@
         <v>2008779.6560113581</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1994,7 +1988,7 @@
         <v>2263478.976617225</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2002,7 +1996,7 @@
         <v>1802663.0673283252</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2010,7 +2004,7 @@
         <v>1545078.9807206674</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2018,7 +2012,7 @@
         <v>2001289.2846407986</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2026,7 +2020,7 @@
         <v>2348803.2827445017</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2034,7 +2028,7 @@
         <v>2684423.0906548309</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2042,7 +2036,7 @@
         <v>2050526.5093742481</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2050,7 +2044,7 @@
         <v>1664321.5142441341</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2058,7 +2052,7 @@
         <v>1368740.3326246841</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2066,7 +2060,7 @@
         <v>2618228.5768152177</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2074,7 +2068,7 @@
         <v>2917258.9577595112</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2082,7 +2076,7 @@
         <v>2909275.1676287227</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2092,10 +2086,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2104,30 +2098,31 @@
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -2136,362 +2131,482 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="D7">
         <v>10.210000000000001</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="D8">
         <v>8.7799999999999994</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="D9">
         <v>0.28000000000000003</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="D10">
         <v>7.24</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="D11">
         <v>0.49</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="D12">
         <v>0.39</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D13">
         <v>533.6</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="D14" s="2">
         <v>3.2</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D15" s="2">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="D16">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D17" s="2">
         <v>1.7799999999999999E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="D18" s="2">
         <v>2.5999999999999999E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D19" s="2">
         <v>1.307E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="D20" s="2">
         <v>1.23E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="D21" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="D22" s="2">
         <v>1.27E-4</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D23" s="2">
         <v>0.45</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="D24" s="2">
         <v>0.08</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="D25" s="2">
         <v>3188</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="D26" s="2">
         <v>74100</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="D27" s="2">
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="D28" s="2">
         <v>0.6</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>24</v>
+      </c>
+      <c r="F28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="2">
+        <v>22.7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="2">
+        <v>22.66</v>
+      </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" xr:uid="{1BEEAAE5-578D-44C2-8322-A37BC3502685}"/>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{1BEEAAE5-578D-44C2-8322-A37BC3502685}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
something is wrong with irrigation electification
</commit_message>
<xml_diff>
--- a/R/data_refs/refbyhand_fuel.xlsx
+++ b/R/data_refs/refbyhand_fuel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_refs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D01BDDC-281F-4CD0-B0B3-144AC23CB6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D55364-4CD9-4137-85C9-8430D5487D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="energy" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="electric-by-state" sheetId="5" r:id="rId4"/>
     <sheet name="combustion-co2" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="108">
   <si>
     <t>fuel_type</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>lb/kwh</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Miles_per_gallon_gasoline_equivalent</t>
   </si>
 </sst>
 </file>
@@ -912,11 +915,10 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1278,7 +1280,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1286,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,7 +1347,7 @@
       <c r="D7">
         <v>0.13800000000000001</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1362,81 +1364,81 @@
       <c r="D8">
         <v>0.125</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>43</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>21</v>
+        <v>3.6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10">
-        <v>9.4</v>
-      </c>
-      <c r="E10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11">
-        <v>39.6</v>
-      </c>
-      <c r="E11" s="3" t="s">
+        <v>9.4</v>
+      </c>
+      <c r="E11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D12">
-        <v>39.020000000000003</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>32</v>
+        <v>39.6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
@@ -1445,26 +1447,43 @@
         <v>28</v>
       </c>
       <c r="D13">
-        <v>34.56</v>
-      </c>
-      <c r="E13" s="3" t="s">
+        <v>39.020000000000003</v>
+      </c>
+      <c r="E13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
       </c>
       <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>34.56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>3.6</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E15" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1613,7 +1632,6 @@
       <c r="D7">
         <v>237724</v>
       </c>
-      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1639,7 +1657,7 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>1751558.4793751165</v>
       </c>
     </row>
@@ -1664,418 +1682,418 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>2560784.2462715139</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>2042826.4776977412</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>2315928.6631540433</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>2053129.1331972515</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>1751558.4793751165</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>2498583.5819126591</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>1810185.6120852982</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>3480873.5784830092</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>2708970.6732206871</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>2368074.0208908846</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>2167974.2159522544</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>3421434.3534036186</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>2112887.4540301901</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>1361645.1097872243</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>1920722.3191254092</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>2887203.9595537884</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>1978660.5696144833</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>3009020.9726553056</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>2545956.2017373675</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>2275870.0673133023</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>2077944.8014844544</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>2349305.5831553484</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>2313246.6291803513</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>2165363.8588073915</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>2728262.7735934332</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>2319164.5749160685</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>2177451.1085846755</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>2010853.1742216183</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>2591179.0138278934</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>2284335.8700390221</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>1692016.9903794336</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>1799491.3032962172</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>2659886.7605724195</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>2047657.9433959115</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>1814360.7201097221</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>2607767.1673954516</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>2128680.6405651919</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>1429694.3177147498</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>2008779.6560113581</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>2263478.976617225</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>1802663.0673283252</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>1545078.9807206674</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>2001289.2846407986</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>2348803.2827445017</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>2684423.0906548309</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>2050526.5093742481</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>1664321.5142441341</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>1368740.3326246841</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>2618228.5768152177</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>2917258.9577595112</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="6">
+      <c r="A57" s="5">
         <v>2909275.1676287227</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2088,7 +2106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed up energy and scenario things
</commit_message>
<xml_diff>
--- a/R/data_refs/refbyhand_fuel.xlsx
+++ b/R/data_refs/refbyhand_fuel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_refs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D55364-4CD9-4137-85C9-8430D5487D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B63D865-B204-4B3F-BC3F-7D0809D77A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3705" yWindow="3480" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="energy" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="electric-by-state" sheetId="5" r:id="rId4"/>
     <sheet name="combustion-co2" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="109">
   <si>
     <t>fuel_type</t>
   </si>
@@ -147,12 +147,6 @@
     <t>greet</t>
   </si>
   <si>
-    <t xml:space="preserve">line 263 from 'petroleum' tab (feedstock + fuel) </t>
-  </si>
-  <si>
-    <t>line 541 from 'electric' tab, column G (CA specific value)</t>
-  </si>
-  <si>
     <t>AK</t>
   </si>
   <si>
@@ -361,6 +355,15 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Miles_per_gallon_gasoline_equivalent</t>
+  </si>
+  <si>
+    <t>line 541 from 'electric' tab, column G (CA specific value; 1,754,558)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line 263 from 'petroleum' tab (CA feedstock (44,763) + CA fuel (diesel &gt; gas) </t>
+  </si>
+  <si>
+    <t>also looked at the eqn in Results tab for electricity AN14, they add fuel and feedstock together, but subtract 1,000,000 and get 1,072,402? Used that for now</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1382,7 +1385,7 @@
         <v>3.6</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1496,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC62357-0511-4CA3-B251-33E17DB7C578}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,10 +1579,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF36B0A1-B092-49AF-918A-1D20B104DADF}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,12 +1597,17 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1658,7 +1666,25 @@
         <v>34</v>
       </c>
       <c r="D9" s="3">
-        <v>1751558.4793751165</v>
+        <v>1072402</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f>1*3.3*0.23</f>
+        <v>0.75900000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f>1*4.2*0.21</f>
+        <v>0.88200000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f>1.1*1.07</f>
+        <v>1.1770000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1678,15 +1704,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1694,7 +1720,7 @@
         <v>2560784.2462715139</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1702,7 +1728,7 @@
         <v>2042826.4776977412</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1710,7 +1736,7 @@
         <v>2315928.6631540433</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1718,7 +1744,7 @@
         <v>2053129.1331972515</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1726,7 +1752,7 @@
         <v>1751558.4793751165</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1734,7 +1760,7 @@
         <v>2498583.5819126591</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1742,7 +1768,7 @@
         <v>1810185.6120852982</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1750,7 +1776,7 @@
         <v>3480873.5784830092</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1758,7 +1784,7 @@
         <v>2708970.6732206871</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1766,7 +1792,7 @@
         <v>2368074.0208908846</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1774,7 +1800,7 @@
         <v>2167974.2159522544</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1782,7 +1808,7 @@
         <v>3421434.3534036186</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1790,7 +1816,7 @@
         <v>2112887.4540301901</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1798,7 +1824,7 @@
         <v>1361645.1097872243</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1806,7 +1832,7 @@
         <v>1920722.3191254092</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1814,7 +1840,7 @@
         <v>2887203.9595537884</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1822,7 +1848,7 @@
         <v>1978660.5696144833</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1830,7 +1856,7 @@
         <v>3009020.9726553056</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1838,7 +1864,7 @@
         <v>2545956.2017373675</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1846,7 +1872,7 @@
         <v>2275870.0673133023</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1854,7 +1880,7 @@
         <v>2077944.8014844544</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1862,7 +1888,7 @@
         <v>2349305.5831553484</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1870,7 +1896,7 @@
         <v>2313246.6291803513</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1878,7 +1904,7 @@
         <v>2165363.8588073915</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1886,7 +1912,7 @@
         <v>2728262.7735934332</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1894,7 +1920,7 @@
         <v>2319164.5749160685</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1902,7 +1928,7 @@
         <v>2177451.1085846755</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1910,7 +1936,7 @@
         <v>2010853.1742216183</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1918,7 +1944,7 @@
         <v>2591179.0138278934</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1926,7 +1952,7 @@
         <v>2284335.8700390221</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1934,7 +1960,7 @@
         <v>1692016.9903794336</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1942,7 +1968,7 @@
         <v>1799491.3032962172</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1950,7 +1976,7 @@
         <v>2659886.7605724195</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1958,7 +1984,7 @@
         <v>2047657.9433959115</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1966,7 +1992,7 @@
         <v>1814360.7201097221</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1974,7 +2000,7 @@
         <v>2607767.1673954516</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1982,7 +2008,7 @@
         <v>2128680.6405651919</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1990,7 +2016,7 @@
         <v>1429694.3177147498</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1998,7 +2024,7 @@
         <v>2008779.6560113581</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2006,7 +2032,7 @@
         <v>2263478.976617225</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2014,7 +2040,7 @@
         <v>1802663.0673283252</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2022,7 +2048,7 @@
         <v>1545078.9807206674</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2030,7 +2056,7 @@
         <v>2001289.2846407986</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2038,7 +2064,7 @@
         <v>2348803.2827445017</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2046,7 +2072,7 @@
         <v>2684423.0906548309</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2054,7 +2080,7 @@
         <v>2050526.5093742481</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2062,7 +2088,7 @@
         <v>1664321.5142441341</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2070,7 +2096,7 @@
         <v>1368740.3326246841</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2078,7 +2104,7 @@
         <v>2618228.5768152177</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2086,7 +2112,7 @@
         <v>2917258.9577595112</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2094,7 +2120,7 @@
         <v>2909275.1676287227</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2140,7 +2166,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -2160,10 +2186,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D7">
         <v>10.210000000000001</v>
@@ -2180,10 +2206,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D8">
         <v>8.7799999999999994</v>
@@ -2200,10 +2226,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D9">
         <v>0.28000000000000003</v>
@@ -2220,10 +2246,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10">
         <v>7.24</v>
@@ -2240,10 +2266,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D11">
         <v>0.49</v>
@@ -2260,10 +2286,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D12">
         <v>0.39</v>
@@ -2280,10 +2306,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D13">
         <v>533.6</v>
@@ -2300,10 +2326,10 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D14" s="2">
         <v>3.2</v>
@@ -2320,10 +2346,10 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D15" s="2">
         <v>0.6</v>
@@ -2337,10 +2363,10 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D16">
         <v>2.7</v>
@@ -2354,10 +2380,10 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D17" s="2">
         <v>1.7799999999999999E-4</v>
@@ -2371,10 +2397,10 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D18" s="2">
         <v>2.5999999999999999E-3</v>
@@ -2388,10 +2414,10 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D19" s="2">
         <v>1.307E-3</v>
@@ -2405,10 +2431,10 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D20" s="2">
         <v>1.23E-3</v>
@@ -2422,10 +2448,10 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D21" s="2">
         <v>2.0000000000000001E-4</v>
@@ -2439,10 +2465,10 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D22" s="2">
         <v>1.27E-4</v>
@@ -2456,10 +2482,10 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D23" s="2">
         <v>0.45</v>
@@ -2476,10 +2502,10 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D24" s="2">
         <v>0.08</v>
@@ -2496,10 +2522,10 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D25" s="2">
         <v>3188</v>
@@ -2516,10 +2542,10 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D26" s="2">
         <v>74100</v>
@@ -2536,10 +2562,10 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D27" s="2">
         <v>10</v>
@@ -2556,10 +2582,10 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D28" s="2">
         <v>0.6</v>
@@ -2576,16 +2602,16 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D29" s="2">
         <v>22.7</v>
       </c>
       <c r="E29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2593,16 +2619,16 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D30" s="2">
         <v>22.66</v>
       </c>
       <c r="E30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2610,16 +2636,16 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D31" s="2">
         <v>0.56999999999999995</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>